<commit_message>
Use of `,` instead of `|` to sep multi value types (#989)
</commit_message>
<xml_diff>
--- a/tests/data/information-unknown-value-type.xlsx
+++ b/tests/data/information-unknown-value-type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E991277D-0AFD-BE46-B937-057E10BDFC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B132B16-1EC0-8247-AD4E-67E1C13AA915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="3480" windowWidth="28520" windowHeight="17920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5440" yWindow="3480" windowWidth="28520" windowHeight="17920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -132,16 +132,7 @@
     <t>operator</t>
   </si>
   <si>
-    <t>string | Person</t>
-  </si>
-  <si>
-    <t>Point | Bboa | Line</t>
-  </si>
-  <si>
     <t>creationTime</t>
-  </si>
-  <si>
-    <t>string | date</t>
   </si>
   <si>
     <t>space</t>
@@ -151,6 +142,15 @@
   </si>
   <si>
     <t>BadModel</t>
+  </si>
+  <si>
+    <t>Point, Bboa, Line</t>
+  </si>
+  <si>
+    <t>string, Person</t>
+  </si>
+  <si>
+    <t>string, date</t>
   </si>
 </sst>
 </file>
@@ -747,7 +747,7 @@
   </sheetPr>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -841,7 +841,7 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>31</v>
@@ -870,10 +870,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -8619,8 +8619,8 @@
   </sheetPr>
   <dimension ref="A1:U912"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8757,7 +8757,7 @@
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E6" s="22">
         <v>1</v>
@@ -8797,7 +8797,7 @@
       </c>
       <c r="C8" s="21"/>
       <c r="D8" s="21" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E8" s="22">
         <v>1</v>
@@ -8813,11 +8813,11 @@
         <v>4</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E9" s="22">
         <v>1</v>

</xml_diff>